<commit_message>
- Add Pregnancy Surveillance feature:   - Add Pregnancy Follow-up Visit database tables through database migration   - Add new parameters to the system for Number of Ante/Postpartum visits   - Add workflow services and controllers for pregnancy surveillance   - Update pregnancy surveillance summary variables through PregnancyRegistrationService, PregnancyOutcomeService, PregnancyVisitService - Update Household Relocation ODK Extension form (labels fix)
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/household_relocation_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/household_relocation_ext.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27645" windowHeight="11985" activeTab="2"/>
+    <workbookView windowWidth="18045" windowHeight="6120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,7 @@
     <t>version</t>
   </si>
   <si>
-    <t>HDS Change Head of Household Extension</t>
+    <t>HDS Household Relocation Extension Form</t>
   </si>
   <si>
     <t>household_relocation_ext</t>
@@ -361,8 +361,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -407,9 +407,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,69 +430,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,8 +447,37 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -522,8 +490,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,8 +520,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,7 +530,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,13 +578,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,49 +626,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,19 +668,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,7 +722,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,43 +740,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -740,25 +752,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,11 +796,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -816,6 +822,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -837,11 +854,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -849,23 +864,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -873,155 +873,155 @@
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3688,13 +3688,13 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.54166666666667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="32.9083333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="53" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.0416666666667" style="1" customWidth="1"/>

</xml_diff>